<commit_message>
vy đã thay đổi
</commit_message>
<xml_diff>
--- a/Lop NM03.xlsx
+++ b/Lop NM03.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>LỚP NHẬP MÔN 03</t>
   </si>
@@ -64,13 +64,16 @@
   </si>
   <si>
     <t>Đỗ Thị Hồng Vy</t>
+  </si>
+  <si>
+    <t>dohongvytn3105@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +84,14 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,14 +114,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -413,7 +427,7 @@
   <dimension ref="C4:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,12 +464,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>4</v>
       </c>
@@ -463,12 +477,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>5</v>
       </c>
@@ -476,7 +490,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>6</v>
       </c>
@@ -485,6 +499,9 @@
       </c>
       <c r="E32">
         <v>1655533908</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
@@ -498,8 +515,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F32" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
vu đã tahy đổi
</commit_message>
<xml_diff>
--- a/Lop NM03.xlsx
+++ b/Lop NM03.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>LỚP NHẬP MÔN 03</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>dohongvytn3105@gmail.com</t>
+  </si>
+  <si>
+    <t>Trịnh Đình Vũ</t>
+  </si>
+  <si>
+    <t>trinhvu21899@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -426,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,12 +510,23 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33">
+        <v>961973654</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>8</v>
       </c>
@@ -517,9 +534,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F32" r:id="rId1"/>
+    <hyperlink ref="F33" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>